<commit_message>
Nearly done with first working version
</commit_message>
<xml_diff>
--- a/905_NBYC_Shiny_local/www/TrialData.xlsx
+++ b/905_NBYC_Shiny_local/www/TrialData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>Lantmet</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Plant population adjusted</t>
   </si>
   <si>
-    <t>design</t>
-  </si>
-  <si>
     <t>year</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>Own</t>
   </si>
   <si>
-    <t>Ädelholm</t>
-  </si>
-  <si>
     <t>emergence</t>
   </si>
   <si>
@@ -75,21 +69,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>designText</t>
-  </si>
-  <si>
-    <t>weatherSourceText</t>
-  </si>
-  <si>
-    <t>external_id</t>
-  </si>
-  <si>
-    <t>site</t>
-  </si>
-  <si>
-    <t>siteText</t>
-  </si>
-  <si>
     <t>soil_b</t>
   </si>
   <si>
@@ -183,10 +162,34 @@
     <t>NBR</t>
   </si>
   <si>
-    <t>Skegrie</t>
-  </si>
-  <si>
-    <t>UFO</t>
+    <t>weather_source_text</t>
+  </si>
+  <si>
+    <t>user_text</t>
+  </si>
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>Ädelholm_4</t>
+  </si>
+  <si>
+    <t>Ädelholm_3</t>
+  </si>
+  <si>
+    <t>Ädelholm_2</t>
+  </si>
+  <si>
+    <t>Ädelholm_1</t>
+  </si>
+  <si>
+    <t>field_external_id</t>
+  </si>
+  <si>
+    <t>inputs</t>
+  </si>
+  <si>
+    <t>inputs_text</t>
   </si>
 </sst>
 </file>
@@ -505,178 +508,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ9"/>
+  <dimension ref="A1:AQ10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="15" max="17" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="Y1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Z1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB1" t="s">
         <v>22</v>
       </c>
-      <c r="M1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="AC1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" t="s">
         <v>23</v>
       </c>
-      <c r="O1" t="s">
-        <v>47</v>
-      </c>
-      <c r="P1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>49</v>
-      </c>
-      <c r="R1" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="AF1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" t="s">
-        <v>13</v>
-      </c>
-      <c r="U1" t="s">
-        <v>14</v>
-      </c>
-      <c r="V1" t="s">
+      <c r="AI1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK1" t="s">
         <v>25</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AL1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" t="s">
         <v>26</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AO1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AP1" t="s">
         <v>27</v>
       </c>
-      <c r="Y1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL1" t="s">
+      <c r="AQ1" t="s">
         <v>39</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>51</v>
+      <c r="A2">
+        <f t="shared" ref="A2:A7" si="0">B2*10000+G2+D2*100-200000</f>
+        <v>11501</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B8" si="0">D2*10000+F2+H2*100-200000</f>
-        <v>11501</v>
-      </c>
-      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="str">
+        <f>VLOOKUP(B2,Design!F$1:G$1,2)</f>
+        <v>NBR</v>
+      </c>
+      <c r="D2">
+        <v>2015</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2">
         <v>282131</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="str">
-        <f>VLOOKUP(D2,Design!F$1:G$1,2)</f>
-        <v>Ädelholm</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="str">
-        <f>VLOOKUP(F2,Design!A$1:B$5,2)</f>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="str">
+        <f>VLOOKUP(G2,Design!A$1:B$5,2)</f>
         <v>Basic</v>
       </c>
-      <c r="H2">
-        <v>2015</v>
-      </c>
       <c r="I2">
-        <v>55.75</v>
+        <v>55.662999999999997</v>
       </c>
       <c r="J2">
         <v>20</v>
@@ -783,35 +787,35 @@
       </c>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3">
+      <c r="A3">
         <f t="shared" si="0"/>
         <v>11601</v>
       </c>
-      <c r="C3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="str">
+        <f>VLOOKUP(B3,Design!F$1:G$1,2)</f>
+        <v>NBR</v>
+      </c>
+      <c r="D3">
+        <v>2016</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3">
         <v>282131</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="str">
-        <f>VLOOKUP(D3,Design!F$1:G$1,2)</f>
-        <v>Ädelholm</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="str">
-        <f>VLOOKUP(F3,Design!A$1:B$5,2)</f>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="str">
+        <f>VLOOKUP(G3,Design!A$1:B$5,2)</f>
         <v>Basic</v>
       </c>
-      <c r="H3">
-        <v>2016</v>
-      </c>
       <c r="I3">
-        <v>55.75</v>
+        <v>55.664999999999999</v>
       </c>
       <c r="J3">
         <v>20</v>
@@ -918,35 +922,35 @@
       </c>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4">
+      <c r="A4">
         <f t="shared" si="0"/>
         <v>11701</v>
       </c>
-      <c r="C4">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="str">
+        <f>VLOOKUP(B4,Design!F$1:G$1,2)</f>
+        <v>NBR</v>
+      </c>
+      <c r="D4">
+        <v>2017</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4">
         <v>282131</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="str">
-        <f>VLOOKUP(D4,Design!F$1:G$1,2)</f>
-        <v>Ädelholm</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="str">
-        <f>VLOOKUP(F4,Design!A$1:B$5,2)</f>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="str">
+        <f>VLOOKUP(G4,Design!A$1:B$5,2)</f>
         <v>Basic</v>
       </c>
-      <c r="H4">
-        <v>2017</v>
-      </c>
       <c r="I4">
-        <v>55.75</v>
+        <v>55.667000000000002</v>
       </c>
       <c r="J4">
         <v>20</v>
@@ -1053,35 +1057,35 @@
       </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5">
+      <c r="A5">
         <f t="shared" si="0"/>
         <v>11801</v>
       </c>
-      <c r="C5">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="str">
+        <f>VLOOKUP(B5,Design!F$1:G$1,2)</f>
+        <v>NBR</v>
+      </c>
+      <c r="D5">
+        <v>2018</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5">
         <v>282131</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="str">
-        <f>VLOOKUP(D5,Design!F$1:G$1,2)</f>
-        <v>Ädelholm</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="str">
-        <f>VLOOKUP(F5,Design!A$1:B$5,2)</f>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="str">
+        <f>VLOOKUP(G5,Design!A$1:B$5,2)</f>
         <v>Basic</v>
       </c>
-      <c r="H5">
-        <v>2018</v>
-      </c>
       <c r="I5">
-        <v>55.75</v>
+        <v>55.661000000000001</v>
       </c>
       <c r="J5">
         <v>20</v>
@@ -1188,35 +1192,35 @@
       </c>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6">
+      <c r="A6">
         <f t="shared" si="0"/>
         <v>11901</v>
       </c>
-      <c r="C6">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="str">
+        <f>VLOOKUP(B6,Design!F$1:G$1,2)</f>
+        <v>NBR</v>
+      </c>
+      <c r="D6">
+        <v>2019</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6">
         <v>282131</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="str">
-        <f>VLOOKUP(D6,Design!F$1:G$1,2)</f>
-        <v>Ädelholm</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="str">
-        <f>VLOOKUP(F6,Design!A$1:B$5,2)</f>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="str">
+        <f>VLOOKUP(G6,Design!A$1:B$5,2)</f>
         <v>Basic</v>
       </c>
-      <c r="H6">
-        <v>2019</v>
-      </c>
       <c r="I6">
-        <v>55.75</v>
+        <v>55.662999999999997</v>
       </c>
       <c r="J6">
         <v>20</v>
@@ -1323,35 +1327,35 @@
       </c>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7">
+      <c r="A7">
         <f t="shared" si="0"/>
         <v>12001</v>
       </c>
-      <c r="C7">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="str">
+        <f>VLOOKUP(B7,Design!F$1:G$1,2)</f>
+        <v>NBR</v>
+      </c>
+      <c r="D7">
+        <v>2020</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7">
         <v>282131</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="str">
-        <f>VLOOKUP(D7,Design!F$1:G$1,2)</f>
-        <v>Ädelholm</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="str">
-        <f>VLOOKUP(F7,Design!A$1:B$5,2)</f>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="str">
+        <f>VLOOKUP(G7,Design!A$1:B$5,2)</f>
         <v>Basic</v>
       </c>
-      <c r="H7">
-        <v>2020</v>
-      </c>
       <c r="I7">
-        <v>55.75</v>
+        <v>55.664999999999999</v>
       </c>
       <c r="J7">
         <v>20</v>
@@ -1458,35 +1462,35 @@
       </c>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>51</v>
+      <c r="A8">
+        <f t="shared" ref="A8:A9" si="1">B8*10000+G8+D8*100-200000</f>
+        <v>12101</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
-        <v>12101</v>
-      </c>
-      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="str">
+        <f>VLOOKUP(B8,Design!F$1:G$1,2)</f>
+        <v>NBR</v>
+      </c>
+      <c r="D8">
+        <v>2021</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8">
         <v>282131</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="str">
-        <f>VLOOKUP(D8,Design!F$1:G$1,2)</f>
-        <v>Ädelholm</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="str">
-        <f>VLOOKUP(F8,Design!A$1:B$5,2)</f>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="str">
+        <f>VLOOKUP(G8,Design!A$1:B$5,2)</f>
         <v>Basic</v>
       </c>
-      <c r="H8">
-        <v>2021</v>
-      </c>
       <c r="I8">
-        <v>55.75</v>
+        <v>55.667000000000002</v>
       </c>
       <c r="J8">
         <v>20</v>
@@ -1593,39 +1597,41 @@
       </c>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>52</v>
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>12201</v>
       </c>
       <c r="B9">
-        <v>22201</v>
-      </c>
-      <c r="C9">
-        <v>123456</v>
+        <v>1</v>
+      </c>
+      <c r="C9" t="str">
+        <f>VLOOKUP(B9,Design!F$1:G$1,2)</f>
+        <v>NBR</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="str">
-        <f>VLOOKUP(F9,Design!A$1:B$5,2)</f>
+        <v>282131</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="str">
+        <f>VLOOKUP(G9,Design!A$1:B$5,2)</f>
         <v>Basic</v>
       </c>
-      <c r="H9">
-        <v>2022</v>
-      </c>
       <c r="I9">
-        <v>55.401998616212801</v>
+        <v>55.661000000000001</v>
       </c>
       <c r="J9">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K9">
-        <v>4</v>
+        <v>2.4</v>
       </c>
       <c r="L9">
         <v>1</v>
@@ -1635,16 +1641,16 @@
         <v>Lantmet</v>
       </c>
       <c r="N9">
-        <v>40142</v>
+        <v>40141</v>
       </c>
       <c r="O9" s="1">
         <v>44645</v>
       </c>
       <c r="P9" s="1">
-        <v>44849</v>
+        <v>44866</v>
       </c>
       <c r="Q9" s="1">
-        <v>44656</v>
+        <v>44659</v>
       </c>
       <c r="R9">
         <v>0</v>
@@ -1722,6 +1728,141 @@
         <v>0</v>
       </c>
       <c r="AQ9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <f>B10*10000+G10+D10*100-200000</f>
+        <v>12301</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="str">
+        <f>VLOOKUP(B10,Design!F$1:G$1,2)</f>
+        <v>NBR</v>
+      </c>
+      <c r="D10">
+        <v>2023</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <v>282131</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="str">
+        <f>VLOOKUP(G10,Design!A$1:B$5,2)</f>
+        <v>Basic</v>
+      </c>
+      <c r="I10">
+        <v>55.662999999999997</v>
+      </c>
+      <c r="J10">
+        <v>20</v>
+      </c>
+      <c r="K10">
+        <v>2.4</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10" t="str">
+        <f>VLOOKUP(L10,Design!C$1:D$2,2)</f>
+        <v>Lantmet</v>
+      </c>
+      <c r="N10">
+        <v>40141</v>
+      </c>
+      <c r="O10" s="1">
+        <v>45023</v>
+      </c>
+      <c r="P10" s="1">
+        <v>45231</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>45033</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>90000</v>
+      </c>
+      <c r="W10">
+        <v>90000</v>
+      </c>
+      <c r="X10">
+        <v>90000</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10">
+        <v>0</v>
+      </c>
+      <c r="AK10">
+        <v>0</v>
+      </c>
+      <c r="AL10">
+        <v>0</v>
+      </c>
+      <c r="AM10">
+        <v>0</v>
+      </c>
+      <c r="AN10">
+        <v>0</v>
+      </c>
+      <c r="AO10">
+        <v>0</v>
+      </c>
+      <c r="AP10">
+        <v>0</v>
+      </c>
+      <c r="AQ10">
         <v>0</v>
       </c>
     </row>
@@ -1734,19 +1875,19 @@
           <x14:formula1>
             <xm:f>Design!$A$1:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F8</xm:sqref>
+          <xm:sqref>G2:G10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Design!$C$1:$C$2</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L8</xm:sqref>
+          <xm:sqref>L2:L10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Design!$F$1</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D8</xm:sqref>
+          <xm:sqref>B2:B8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1758,9 +1899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1784,7 +1923,7 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -1798,7 +1937,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Minor updates, mainly to formatting
</commit_message>
<xml_diff>
--- a/905_NBYC_Shiny_local/www/TrialData.xlsx
+++ b/905_NBYC_Shiny_local/www/TrialData.xlsx
@@ -511,7 +511,7 @@
   <dimension ref="A1:AQ10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -705,7 +705,7 @@
         <v>42309</v>
       </c>
       <c r="Q2" s="1">
-        <v>42118</v>
+        <v>42108</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -834,7 +834,7 @@
         <v>40141</v>
       </c>
       <c r="O3" s="1">
-        <v>42461</v>
+        <v>42470</v>
       </c>
       <c r="P3" s="1">
         <v>42675</v>
@@ -975,7 +975,7 @@
         <v>43040</v>
       </c>
       <c r="Q4" s="1">
-        <v>42850</v>
+        <v>42840</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -1104,13 +1104,13 @@
         <v>40141</v>
       </c>
       <c r="O5" s="1">
-        <v>43191</v>
+        <v>43177</v>
       </c>
       <c r="P5" s="1">
         <v>43405</v>
       </c>
       <c r="Q5" s="1">
-        <v>43215</v>
+        <v>43193</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -1239,13 +1239,13 @@
         <v>40141</v>
       </c>
       <c r="O6" s="1">
-        <v>43556</v>
+        <v>43557</v>
       </c>
       <c r="P6" s="1">
         <v>43770</v>
       </c>
       <c r="Q6" s="1">
-        <v>43580</v>
+        <v>43572</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -1380,7 +1380,7 @@
         <v>44136</v>
       </c>
       <c r="Q7" s="1">
-        <v>43946</v>
+        <v>43935</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -1509,7 +1509,7 @@
         <v>40141</v>
       </c>
       <c r="O8" s="1">
-        <v>44287</v>
+        <v>44301</v>
       </c>
       <c r="P8" s="1">
         <v>44501</v>

</xml_diff>